<commit_message>
Added first results wit RTS/CTS
</commit_message>
<xml_diff>
--- a/new_results/all_results_2.xlsx
+++ b/new_results/all_results_2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folder\Studia-materialy_i_ksiazki\magisterka\MS_project2\new_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MetodySymulacyjne\MS_project2\new_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB48B162-7E48-4DB2-A47F-EA2FCF2BC79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23550" yWindow="-6525" windowWidth="23655" windowHeight="15840" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-23554" yWindow="-6523" windowWidth="23657" windowHeight="15840" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="razem" sheetId="3" r:id="rId1"/>
@@ -21,19 +22,28 @@
     <sheet name="legacy thr no ampdu" sheetId="7" r:id="rId7"/>
     <sheet name="ax delay no ampdu" sheetId="8" r:id="rId8"/>
     <sheet name="legacy delay no ampdu" sheetId="9" r:id="rId9"/>
+    <sheet name="RTS_CTS" sheetId="14" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,7 +132,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -850,7 +859,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -882,7 +890,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -890,6 +897,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1445,7 +1453,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1453,6 +1460,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2008,7 +2016,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2016,6 +2023,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2571,7 +2579,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2579,6 +2586,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3388,7 +3396,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3420,7 +3427,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3428,6 +3434,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3510,7 +3517,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4069,7 +4075,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4101,7 +4106,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4109,6 +4113,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4191,7 +4196,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4760,7 +4764,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4792,7 +4795,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4800,6 +4802,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5355,7 +5358,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5363,6 +5365,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5912,7 +5915,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5920,6 +5922,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6486,7 +6489,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -6494,6 +6496,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7049,7 +7052,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7057,6 +7059,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7612,7 +7615,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7620,6 +7622,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -14346,7 +14349,7 @@
         <xdr:cNvPr id="4" name="Wykres 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974CB4B7-82F1-4D53-956F-185AA43BCD5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14382,7 +14385,7 @@
         <xdr:cNvPr id="5" name="Wykres 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974CB4B7-82F1-4D53-956F-185AA43BCD5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14420,7 +14423,7 @@
         <xdr:cNvPr id="6" name="Wykres 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974CB4B7-82F1-4D53-956F-185AA43BCD5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14458,7 +14461,7 @@
         <xdr:cNvPr id="7" name="Wykres 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974CB4B7-82F1-4D53-956F-185AA43BCD5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14501,7 +14504,7 @@
         <xdr:cNvPr id="3" name="Wykres 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED4780-272E-482C-8D99-52ACFF97DC63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14542,7 +14545,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C67758F-AE5E-49A6-919F-5C5DEA72AF04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14583,7 +14586,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE1BB197-2C06-402F-8FCA-BE69B4D0E8E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14624,7 +14627,7 @@
         <xdr:cNvPr id="3" name="Wykres 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CAD6528-21F3-4F98-BC06-DCDDE58E2E6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14665,7 +14668,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED4780-272E-482C-8D99-52ACFF97DC63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14708,7 +14711,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C67758F-AE5E-49A6-919F-5C5DEA72AF04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14751,7 +14754,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED4780-272E-482C-8D99-52ACFF97DC63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14794,7 +14797,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED4780-272E-482C-8D99-52ACFF97DC63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15079,7 +15082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
@@ -15093,8 +15096,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499DB053-101B-4237-9B7C-8A425DFCA3A6}">
+  <dimension ref="B3:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>333</v>
+      </c>
+      <c r="D3">
+        <v>334</v>
+      </c>
+      <c r="E3">
+        <v>335</v>
+      </c>
+      <c r="F3">
+        <v>336</v>
+      </c>
+      <c r="G3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="e">
+        <f t="shared" ref="H4:H6" si="0">AVERAGE(C4:G4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" t="e">
+        <f t="shared" ref="I4:I6" si="1">STDEV(C4:G4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" t="e">
+        <f t="shared" ref="J4:J6" si="2">_xlfn.CONFIDENCE.NORM(0.05, I4, COUNTA(C4:G4))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="H5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="H6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>398.99234772000011</v>
+      </c>
+      <c r="E7">
+        <v>349.52111785999978</v>
+      </c>
+      <c r="F7">
+        <v>425.85943592000001</v>
+      </c>
+      <c r="G7">
+        <v>428.08839937000022</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(C7:G7)</f>
+        <v>400.61532521750001</v>
+      </c>
+      <c r="I7">
+        <f>STDEV(C7:G7)</f>
+        <v>36.538960986858363</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, I7, COUNTA(C7:G7))</f>
+        <v>35.807523783378244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15804,7 +15919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16481,7 +16596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17188,7 +17303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17901,7 +18016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18623,7 +18738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19333,7 +19448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20055,10 +20170,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>

</xml_diff>